<commit_message>
homeworks from 4 students
</commit_message>
<xml_diff>
--- a/软件质量保证听课名单.xlsx
+++ b/软件质量保证听课名单.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="105" windowWidth="7515" windowHeight="4455"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="软件质量保证听课名单" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="90">
   <si>
     <t>学号</t>
   </si>
@@ -260,31 +260,51 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>N</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>假条</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>请假</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>请假</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>n</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>N</t>
+    <t>?</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>y</t>
+    <t>作业</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>假条</t>
+    <t>作业成绩</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>qingjia</t>
+    <t>n</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -934,7 +954,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1008,7 +1028,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1043,7 +1062,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1219,22 +1237,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="O36" sqref="O36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="6" max="6" width="8.375" customWidth="1"/>
+    <col min="6" max="6" width="8.625" customWidth="1"/>
     <col min="7" max="7" width="9" hidden="1" customWidth="1"/>
     <col min="9" max="9" width="8.125" customWidth="1"/>
     <col min="10" max="10" width="9" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +1275,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1">
-        <v>42057</v>
+        <v>42085</v>
       </c>
       <c r="I1" s="1">
         <v>42092</v>
@@ -1274,8 +1292,17 @@
       <c r="M1" s="1">
         <v>42134</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+      <c r="N1" s="1">
+        <v>42141</v>
+      </c>
+      <c r="O1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2">
         <v>13126159</v>
       </c>
@@ -1292,7 +1319,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16">
       <c r="A3">
         <v>14126072</v>
       </c>
@@ -1309,10 +1336,10 @@
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4">
         <v>14126074</v>
       </c>
@@ -1329,10 +1356,10 @@
         <v>10</v>
       </c>
       <c r="M4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5">
         <v>14126075</v>
       </c>
@@ -1349,10 +1376,10 @@
         <v>10</v>
       </c>
       <c r="M5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6">
         <v>14126077</v>
       </c>
@@ -1369,10 +1396,10 @@
         <v>10</v>
       </c>
       <c r="M6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7">
         <v>14126080</v>
       </c>
@@ -1389,10 +1416,10 @@
         <v>10</v>
       </c>
       <c r="M7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8">
         <v>14126085</v>
       </c>
@@ -1409,10 +1436,10 @@
         <v>10</v>
       </c>
       <c r="M8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9">
         <v>14126086</v>
       </c>
@@ -1429,16 +1456,16 @@
         <v>10</v>
       </c>
       <c r="I9" t="s">
-        <v>83</v>
-      </c>
-      <c r="K9" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="M9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="N9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
       <c r="A10">
         <v>14126090</v>
       </c>
@@ -1455,10 +1482,10 @@
         <v>10</v>
       </c>
       <c r="M10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
       <c r="A11">
         <v>14126092</v>
       </c>
@@ -1475,10 +1502,10 @@
         <v>10</v>
       </c>
       <c r="M11" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
       <c r="A12">
         <v>14126095</v>
       </c>
@@ -1494,11 +1521,17 @@
       <c r="E12" t="s">
         <v>10</v>
       </c>
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
       <c r="M12" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="N12" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
       <c r="A13">
         <v>14126097</v>
       </c>
@@ -1518,10 +1551,10 @@
         <v>77</v>
       </c>
       <c r="M13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
       <c r="A14">
         <v>14126099</v>
       </c>
@@ -1538,10 +1571,10 @@
         <v>10</v>
       </c>
       <c r="M14" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
       <c r="A15">
         <v>14126100</v>
       </c>
@@ -1557,11 +1590,14 @@
       <c r="E15" t="s">
         <v>10</v>
       </c>
+      <c r="H15" t="s">
+        <v>89</v>
+      </c>
       <c r="M15" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
       <c r="A16">
         <v>14126101</v>
       </c>
@@ -1578,10 +1614,10 @@
         <v>10</v>
       </c>
       <c r="M16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>14126103</v>
       </c>
@@ -1597,14 +1633,17 @@
       <c r="E17" t="s">
         <v>10</v>
       </c>
+      <c r="H17" t="s">
+        <v>89</v>
+      </c>
       <c r="I17" t="s">
         <v>77</v>
       </c>
       <c r="M17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>14126104</v>
       </c>
@@ -1620,11 +1659,14 @@
       <c r="E18" t="s">
         <v>10</v>
       </c>
+      <c r="H18" t="s">
+        <v>89</v>
+      </c>
       <c r="M18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>14126106</v>
       </c>
@@ -1640,11 +1682,17 @@
       <c r="E19" t="s">
         <v>10</v>
       </c>
+      <c r="H19" t="s">
+        <v>89</v>
+      </c>
       <c r="M19" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="N19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>14126109</v>
       </c>
@@ -1661,13 +1709,13 @@
         <v>10</v>
       </c>
       <c r="L20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>14126112</v>
       </c>
@@ -1684,10 +1732,10 @@
         <v>10</v>
       </c>
       <c r="M21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>14126115</v>
       </c>
@@ -1704,10 +1752,10 @@
         <v>10</v>
       </c>
       <c r="M22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>14126116</v>
       </c>
@@ -1724,10 +1772,10 @@
         <v>10</v>
       </c>
       <c r="M23" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>14126117</v>
       </c>
@@ -1744,10 +1792,13 @@
         <v>10</v>
       </c>
       <c r="M24" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="O24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25">
         <v>14126118</v>
       </c>
@@ -1764,10 +1815,10 @@
         <v>10</v>
       </c>
       <c r="M25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26">
         <v>14126119</v>
       </c>
@@ -1787,10 +1838,10 @@
         <v>77</v>
       </c>
       <c r="M26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27">
         <v>14126121</v>
       </c>
@@ -1806,11 +1857,14 @@
       <c r="E27" t="s">
         <v>10</v>
       </c>
+      <c r="H27" t="s">
+        <v>89</v>
+      </c>
       <c r="M27" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15">
       <c r="A28">
         <v>14126123</v>
       </c>
@@ -1826,6 +1880,9 @@
       <c r="E28" t="s">
         <v>10</v>
       </c>
+      <c r="H28" t="s">
+        <v>89</v>
+      </c>
       <c r="I28" t="s">
         <v>77</v>
       </c>
@@ -1833,10 +1890,10 @@
         <v>78</v>
       </c>
       <c r="M28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29">
         <v>14126126</v>
       </c>
@@ -1853,10 +1910,10 @@
         <v>10</v>
       </c>
       <c r="M29" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30">
         <v>14126128</v>
       </c>
@@ -1872,14 +1929,17 @@
       <c r="E30" t="s">
         <v>10</v>
       </c>
+      <c r="H30" t="s">
+        <v>89</v>
+      </c>
       <c r="I30" t="s">
         <v>77</v>
       </c>
       <c r="M30" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31">
         <v>14126131</v>
       </c>
@@ -1896,10 +1956,10 @@
         <v>10</v>
       </c>
       <c r="M31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32">
         <v>14126132</v>
       </c>
@@ -1915,11 +1975,14 @@
       <c r="E32" t="s">
         <v>10</v>
       </c>
+      <c r="H32" t="s">
+        <v>89</v>
+      </c>
       <c r="M32" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33">
         <v>14126133</v>
       </c>
@@ -1936,10 +1999,10 @@
         <v>10</v>
       </c>
       <c r="M33" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15">
       <c r="A34">
         <v>14126135</v>
       </c>
@@ -1956,10 +2019,10 @@
         <v>10</v>
       </c>
       <c r="M34" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35">
         <v>14126137</v>
       </c>
@@ -1976,10 +2039,10 @@
         <v>10</v>
       </c>
       <c r="M35" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
       <c r="A36">
         <v>14126138</v>
       </c>
@@ -1996,10 +2059,16 @@
         <v>10</v>
       </c>
       <c r="M36" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="N36" t="s">
+        <v>85</v>
+      </c>
+      <c r="O36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37">
         <v>14126140</v>
       </c>
@@ -2016,10 +2085,10 @@
         <v>10</v>
       </c>
       <c r="M37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38">
         <v>14126141</v>
       </c>
@@ -2036,10 +2105,10 @@
         <v>10</v>
       </c>
       <c r="M38" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39">
         <v>14126142</v>
       </c>
@@ -2056,10 +2125,10 @@
         <v>10</v>
       </c>
       <c r="M39" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40">
         <v>14126143</v>
       </c>
@@ -2075,11 +2144,14 @@
       <c r="E40" t="s">
         <v>10</v>
       </c>
+      <c r="H40" t="s">
+        <v>89</v>
+      </c>
       <c r="M40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41">
         <v>14126145</v>
       </c>
@@ -2096,10 +2168,10 @@
         <v>10</v>
       </c>
       <c r="M41" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15">
       <c r="A42">
         <v>14126146</v>
       </c>
@@ -2115,11 +2187,14 @@
       <c r="E42" t="s">
         <v>10</v>
       </c>
+      <c r="H42" t="s">
+        <v>89</v>
+      </c>
       <c r="M42" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="A43">
         <v>14126150</v>
       </c>
@@ -2136,10 +2211,10 @@
         <v>10</v>
       </c>
       <c r="M43" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="A44">
         <v>14126151</v>
       </c>
@@ -2156,10 +2231,10 @@
         <v>10</v>
       </c>
       <c r="M44" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15">
       <c r="A45">
         <v>14126157</v>
       </c>
@@ -2176,10 +2251,10 @@
         <v>10</v>
       </c>
       <c r="M45" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15">
       <c r="A46">
         <v>14126158</v>
       </c>
@@ -2196,10 +2271,10 @@
         <v>10</v>
       </c>
       <c r="M46" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15">
       <c r="A47">
         <v>14126162</v>
       </c>
@@ -2216,10 +2291,13 @@
         <v>10</v>
       </c>
       <c r="M47" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="N47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15">
       <c r="A48">
         <v>14126163</v>
       </c>
@@ -2236,10 +2314,10 @@
         <v>10</v>
       </c>
       <c r="M48" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15">
       <c r="A49">
         <v>14126164</v>
       </c>
@@ -2255,11 +2333,14 @@
       <c r="E49" t="s">
         <v>10</v>
       </c>
+      <c r="H49" t="s">
+        <v>89</v>
+      </c>
       <c r="M49" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15">
       <c r="A50">
         <v>14126165</v>
       </c>
@@ -2276,10 +2357,10 @@
         <v>10</v>
       </c>
       <c r="M50" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15">
       <c r="A51">
         <v>14126166</v>
       </c>
@@ -2296,10 +2377,10 @@
         <v>10</v>
       </c>
       <c r="M51" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15">
       <c r="A52">
         <v>14126169</v>
       </c>
@@ -2316,10 +2397,10 @@
         <v>10</v>
       </c>
       <c r="M52" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15">
       <c r="A53">
         <v>14126172</v>
       </c>
@@ -2336,7 +2417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:15">
       <c r="A54">
         <v>14126173</v>
       </c>
@@ -2353,10 +2434,10 @@
         <v>10</v>
       </c>
       <c r="M54" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15">
       <c r="A55">
         <v>14126175</v>
       </c>
@@ -2373,10 +2454,10 @@
         <v>10</v>
       </c>
       <c r="M55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15">
       <c r="A56">
         <v>14126176</v>
       </c>
@@ -2393,10 +2474,13 @@
         <v>10</v>
       </c>
       <c r="M56" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="O56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15">
       <c r="A57">
         <v>14126177</v>
       </c>
@@ -2413,10 +2497,10 @@
         <v>10</v>
       </c>
       <c r="M57" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15">
       <c r="A58">
         <v>14126179</v>
       </c>
@@ -2433,10 +2517,13 @@
         <v>10</v>
       </c>
       <c r="M58" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="N58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15">
       <c r="A59">
         <v>14126181</v>
       </c>
@@ -2453,10 +2540,13 @@
         <v>10</v>
       </c>
       <c r="M59" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+      <c r="O59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15">
       <c r="A60">
         <v>14126185</v>
       </c>
@@ -2473,10 +2563,10 @@
         <v>10</v>
       </c>
       <c r="M60" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15">
       <c r="A61">
         <v>14126186</v>
       </c>
@@ -2493,13 +2583,13 @@
         <v>10</v>
       </c>
       <c r="K61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M61" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15">
       <c r="A62">
         <v>14126187</v>
       </c>
@@ -2519,10 +2609,10 @@
         <v>76</v>
       </c>
       <c r="M62" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15">
       <c r="A63">
         <v>14126188</v>
       </c>
@@ -2539,10 +2629,10 @@
         <v>10</v>
       </c>
       <c r="M63" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15">
       <c r="A64">
         <v>14126192</v>
       </c>
@@ -2559,10 +2649,10 @@
         <v>10</v>
       </c>
       <c r="M64" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
       <c r="A65">
         <v>14126193</v>
       </c>
@@ -2578,11 +2668,14 @@
       <c r="E65" t="s">
         <v>10</v>
       </c>
+      <c r="H65" t="s">
+        <v>89</v>
+      </c>
       <c r="M65" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
       <c r="A66">
         <v>14126196</v>
       </c>
@@ -2602,10 +2695,10 @@
         <v>77</v>
       </c>
       <c r="M66" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.15">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
       <c r="A67">
         <v>14126197</v>
       </c>
@@ -2622,11 +2715,12 @@
         <v>10</v>
       </c>
       <c r="M67" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+3 = 7 total
</commit_message>
<xml_diff>
--- a/软件质量保证听课名单.xlsx
+++ b/软件质量保证听课名单.xlsx
@@ -1240,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="O36" sqref="O36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1318,6 +1318,9 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
+      <c r="O2">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3">
@@ -2522,6 +2525,9 @@
       <c r="N58" t="s">
         <v>85</v>
       </c>
+      <c r="O58">
+        <v>5</v>
+      </c>
     </row>
     <row r="59" spans="1:15">
       <c r="A59">
@@ -2652,7 +2658,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:15">
       <c r="A65">
         <v>14126193</v>
       </c>
@@ -2674,8 +2680,11 @@
       <c r="M65" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="66" spans="1:13">
+      <c r="O65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15">
       <c r="A66">
         <v>14126196</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:15">
       <c r="A67">
         <v>14126197</v>
       </c>

</xml_diff>

<commit_message>
1 more: Liu Tianxiang
</commit_message>
<xml_diff>
--- a/软件质量保证听课名单.xlsx
+++ b/软件质量保证听课名单.xlsx
@@ -1248,8 +1248,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O10" sqref="O10"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1911,6 +1911,9 @@
       <c r="M26" t="s">
         <v>73</v>
       </c>
+      <c r="O26">
+        <v>64</v>
+      </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27">

</xml_diff>

<commit_message>
teaching cal, syllabus, score sheet
</commit_message>
<xml_diff>
--- a/软件质量保证听课名单.xlsx
+++ b/软件质量保证听课名单.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="92">
   <si>
     <t>学号</t>
   </si>
@@ -310,6 +310,10 @@
   </si>
   <si>
     <t>成绩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>总成绩</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1251,21 +1255,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q67"/>
+  <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F67"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="6" max="6" width="8.625" customWidth="1"/>
-    <col min="7" max="7" width="9" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="8.125" customWidth="1"/>
-    <col min="10" max="10" width="9" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" customWidth="1"/>
+    <col min="9" max="9" width="6.75" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1317,8 +1321,11 @@
       <c r="Q1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2">
         <v>13126159</v>
       </c>
@@ -1335,8 +1342,8 @@
         <v>9</v>
       </c>
       <c r="F2">
-        <f>O2+Q2*0.6</f>
-        <v>40</v>
+        <f>(O2+Q2*0.6)*0.96</f>
+        <v>87.36</v>
       </c>
       <c r="O2">
         <v>40</v>
@@ -1344,8 +1351,11 @@
       <c r="P2">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="Q2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3">
         <v>14126072</v>
       </c>
@@ -1362,8 +1372,8 @@
         <v>9</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F66" si="0">O3+Q3*0.6</f>
-        <v>43</v>
+        <f t="shared" ref="F3:F66" si="0">(O3+Q3*0.6)*0.96</f>
+        <v>90.24</v>
       </c>
       <c r="M3" t="s">
         <v>72</v>
@@ -1374,8 +1384,11 @@
       <c r="P3">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="Q3">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>14126074</v>
       </c>
@@ -1393,7 +1406,7 @@
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.24</v>
       </c>
       <c r="M4" t="s">
         <v>72</v>
@@ -1404,8 +1417,11 @@
       <c r="P4">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="Q4">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>14126075</v>
       </c>
@@ -1423,7 +1439,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>92.543999999999997</v>
       </c>
       <c r="M5" t="s">
         <v>72</v>
@@ -1434,8 +1450,11 @@
       <c r="P5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="Q5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>14126077</v>
       </c>
@@ -1453,7 +1472,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="M6" t="s">
         <v>72</v>
@@ -1464,8 +1483,11 @@
       <c r="P6">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="Q6">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>14126080</v>
       </c>
@@ -1483,7 +1505,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>84.47999999999999</v>
       </c>
       <c r="M7" t="s">
         <v>72</v>
@@ -1494,8 +1516,11 @@
       <c r="P7">
         <v>51</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="Q7">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>14126085</v>
       </c>
@@ -1513,7 +1538,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>89.087999999999994</v>
       </c>
       <c r="M8" t="s">
         <v>72</v>
@@ -1524,8 +1549,11 @@
       <c r="P8">
         <v>46</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="Q8">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>14126086</v>
       </c>
@@ -1543,7 +1571,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>88.511999999999986</v>
       </c>
       <c r="I9" t="s">
         <v>73</v>
@@ -1560,8 +1588,11 @@
       <c r="P9">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="Q9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>14126090</v>
       </c>
@@ -1579,7 +1610,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>89.087999999999994</v>
       </c>
       <c r="M10" t="s">
         <v>72</v>
@@ -1590,8 +1621,11 @@
       <c r="P10">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="Q10">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11">
         <v>14126092</v>
       </c>
@@ -1609,7 +1643,7 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>93.11999999999999</v>
       </c>
       <c r="M11" t="s">
         <v>72</v>
@@ -1620,8 +1654,11 @@
       <c r="P11">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:17">
+      <c r="Q11">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12">
         <v>14126095</v>
       </c>
@@ -1639,7 +1676,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>83.711999999999989</v>
       </c>
       <c r="H12" t="s">
         <v>80</v>
@@ -1656,8 +1693,11 @@
       <c r="P12">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:17">
+      <c r="Q12">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13">
         <v>14126097</v>
       </c>
@@ -1675,7 +1715,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>86.015999999999991</v>
       </c>
       <c r="I13" t="s">
         <v>68</v>
@@ -1689,8 +1729,11 @@
       <c r="P13">
         <v>65</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="Q13">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14">
         <v>14126099</v>
       </c>
@@ -1708,7 +1751,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>91.391999999999982</v>
       </c>
       <c r="M14" t="s">
         <v>72</v>
@@ -1719,8 +1762,11 @@
       <c r="P14">
         <v>59</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="Q14">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15">
         <v>14126100</v>
       </c>
@@ -1738,7 +1784,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>83.135999999999996</v>
       </c>
       <c r="H15" t="s">
         <v>80</v>
@@ -1752,8 +1798,11 @@
       <c r="P15">
         <v>39</v>
       </c>
-    </row>
-    <row r="16" spans="1:17">
+      <c r="Q15">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16">
         <v>14126101</v>
       </c>
@@ -1771,7 +1820,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>82.751999999999981</v>
       </c>
       <c r="M16" t="s">
         <v>72</v>
@@ -1782,8 +1831,11 @@
       <c r="P16">
         <v>53</v>
       </c>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17">
         <v>14126103</v>
       </c>
@@ -1801,7 +1853,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>81.215999999999994</v>
       </c>
       <c r="H17" t="s">
         <v>80</v>
@@ -1818,8 +1870,11 @@
       <c r="P17">
         <v>18</v>
       </c>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18">
         <v>14126104</v>
       </c>
@@ -1837,7 +1892,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>79.679999999999993</v>
       </c>
       <c r="H18" t="s">
         <v>80</v>
@@ -1851,8 +1906,11 @@
       <c r="P18">
         <v>34</v>
       </c>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19">
         <v>14126106</v>
       </c>
@@ -1870,7 +1928,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>76.60799999999999</v>
       </c>
       <c r="H19" t="s">
         <v>80</v>
@@ -1887,8 +1945,11 @@
       <c r="P19">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20">
         <v>14126109</v>
       </c>
@@ -1906,7 +1967,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>73.92</v>
       </c>
       <c r="L20" t="s">
         <v>71</v>
@@ -1920,8 +1981,11 @@
       <c r="P20">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21">
         <v>14126112</v>
       </c>
@@ -1939,7 +2003,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.815999999999988</v>
       </c>
       <c r="M21" t="s">
         <v>72</v>
@@ -1950,8 +2014,11 @@
       <c r="P21">
         <v>38</v>
       </c>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22">
         <v>14126115</v>
       </c>
@@ -1969,7 +2036,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>89.087999999999994</v>
       </c>
       <c r="M22" t="s">
         <v>72</v>
@@ -1980,8 +2047,11 @@
       <c r="P22">
         <v>56</v>
       </c>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23">
         <v>14126116</v>
       </c>
@@ -1999,7 +2069,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>77.567999999999998</v>
       </c>
       <c r="M23" t="s">
         <v>72</v>
@@ -2010,8 +2080,11 @@
       <c r="P23">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24">
         <v>14126117</v>
       </c>
@@ -2029,7 +2102,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>93.11999999999999</v>
       </c>
       <c r="M24" t="s">
         <v>72</v>
@@ -2040,8 +2113,11 @@
       <c r="P24">
         <v>2</v>
       </c>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25">
         <v>14126118</v>
       </c>
@@ -2059,7 +2135,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>91.391999999999982</v>
       </c>
       <c r="M25" t="s">
         <v>72</v>
@@ -2070,8 +2146,11 @@
       <c r="P25">
         <v>19</v>
       </c>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26">
         <v>14126119</v>
       </c>
@@ -2089,7 +2168,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>75.071999999999989</v>
       </c>
       <c r="I26" t="s">
         <v>68</v>
@@ -2103,8 +2182,11 @@
       <c r="P26">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27">
         <v>14126121</v>
       </c>
@@ -2122,7 +2204,7 @@
       </c>
       <c r="F27">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>87.744</v>
       </c>
       <c r="H27" t="s">
         <v>80</v>
@@ -2136,8 +2218,11 @@
       <c r="P27">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28">
         <v>14126123</v>
       </c>
@@ -2155,7 +2240,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>26.88</v>
       </c>
       <c r="H28" t="s">
         <v>80</v>
@@ -2170,10 +2255,10 @@
         <v>72</v>
       </c>
       <c r="O28">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29">
         <v>14126126</v>
       </c>
@@ -2191,7 +2276,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.815999999999988</v>
       </c>
       <c r="M29" t="s">
         <v>72</v>
@@ -2202,8 +2287,11 @@
       <c r="P29">
         <v>8</v>
       </c>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30">
         <v>14126128</v>
       </c>
@@ -2221,7 +2309,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="0"/>
-        <v>33</v>
+        <v>76.031999999999982</v>
       </c>
       <c r="H30" t="s">
         <v>80</v>
@@ -2238,8 +2326,11 @@
       <c r="P30">
         <v>62</v>
       </c>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31">
         <v>14126131</v>
       </c>
@@ -2257,7 +2348,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>93.11999999999999</v>
       </c>
       <c r="M31" t="s">
         <v>72</v>
@@ -2268,8 +2359,11 @@
       <c r="P31">
         <v>36</v>
       </c>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32">
         <v>14126132</v>
       </c>
@@ -2287,7 +2381,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>82.56</v>
       </c>
       <c r="H32" t="s">
         <v>80</v>
@@ -2301,8 +2395,11 @@
       <c r="P32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33">
         <v>14126133</v>
       </c>
@@ -2320,7 +2417,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>87.935999999999993</v>
       </c>
       <c r="M33" t="s">
         <v>72</v>
@@ -2331,8 +2428,11 @@
       <c r="P33">
         <v>58</v>
       </c>
-    </row>
-    <row r="34" spans="1:16">
+      <c r="Q33">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17">
       <c r="A34">
         <v>14126135</v>
       </c>
@@ -2350,7 +2450,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>93.11999999999999</v>
       </c>
       <c r="M34" t="s">
         <v>72</v>
@@ -2361,8 +2461,11 @@
       <c r="P34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:16">
+      <c r="Q34">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17">
       <c r="A35">
         <v>14126137</v>
       </c>
@@ -2380,7 +2483,7 @@
       </c>
       <c r="F35">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>91.967999999999989</v>
       </c>
       <c r="M35" t="s">
         <v>72</v>
@@ -2391,8 +2494,11 @@
       <c r="P35">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:16">
+      <c r="Q35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17">
       <c r="A36">
         <v>14126138</v>
       </c>
@@ -2410,7 +2516,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>88.32</v>
       </c>
       <c r="M36" t="s">
         <v>72</v>
@@ -2424,8 +2530,11 @@
       <c r="P36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:16">
+      <c r="Q36">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17">
       <c r="A37">
         <v>14126140</v>
       </c>
@@ -2443,7 +2552,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.24</v>
       </c>
       <c r="M37" t="s">
         <v>72</v>
@@ -2454,8 +2563,11 @@
       <c r="P37">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:16">
+      <c r="Q37">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17">
       <c r="A38">
         <v>14126141</v>
       </c>
@@ -2473,7 +2585,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>86.207999999999998</v>
       </c>
       <c r="M38" t="s">
         <v>72</v>
@@ -2484,8 +2596,11 @@
       <c r="P38">
         <v>35</v>
       </c>
-    </row>
-    <row r="39" spans="1:16">
+      <c r="Q38">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17">
       <c r="A39">
         <v>14126142</v>
       </c>
@@ -2503,7 +2618,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>88.511999999999986</v>
       </c>
       <c r="M39" t="s">
         <v>72</v>
@@ -2514,8 +2629,11 @@
       <c r="P39">
         <v>40</v>
       </c>
-    </row>
-    <row r="40" spans="1:16">
+      <c r="Q39">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17">
       <c r="A40">
         <v>14126143</v>
       </c>
@@ -2533,7 +2651,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>81.984000000000009</v>
       </c>
       <c r="H40" t="s">
         <v>80</v>
@@ -2547,8 +2665,11 @@
       <c r="P40">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:16">
+      <c r="Q40">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17">
       <c r="A41">
         <v>14126145</v>
       </c>
@@ -2566,7 +2687,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>84.47999999999999</v>
       </c>
       <c r="M41" t="s">
         <v>72</v>
@@ -2577,8 +2698,11 @@
       <c r="P41">
         <v>55</v>
       </c>
-    </row>
-    <row r="42" spans="1:16">
+      <c r="Q41">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17">
       <c r="A42">
         <v>14126146</v>
       </c>
@@ -2596,7 +2720,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>83.135999999999996</v>
       </c>
       <c r="H42" t="s">
         <v>80</v>
@@ -2610,8 +2734,11 @@
       <c r="P42">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:16">
+      <c r="Q42">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17">
       <c r="A43">
         <v>14126150</v>
       </c>
@@ -2629,7 +2756,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>91.391999999999982</v>
       </c>
       <c r="M43" t="s">
         <v>72</v>
@@ -2640,8 +2767,11 @@
       <c r="P43">
         <v>52</v>
       </c>
-    </row>
-    <row r="44" spans="1:16">
+      <c r="Q43">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17">
       <c r="A44">
         <v>14126151</v>
       </c>
@@ -2659,7 +2789,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.815999999999988</v>
       </c>
       <c r="M44" t="s">
         <v>72</v>
@@ -2670,8 +2800,11 @@
       <c r="P44">
         <v>22</v>
       </c>
-    </row>
-    <row r="45" spans="1:16">
+      <c r="Q44">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17">
       <c r="A45">
         <v>14126157</v>
       </c>
@@ -2689,7 +2822,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>91.967999999999989</v>
       </c>
       <c r="M45" t="s">
         <v>72</v>
@@ -2700,8 +2833,11 @@
       <c r="P45">
         <v>28</v>
       </c>
-    </row>
-    <row r="46" spans="1:16">
+      <c r="Q45">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17">
       <c r="A46">
         <v>14126158</v>
       </c>
@@ -2719,7 +2855,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>86.784000000000006</v>
       </c>
       <c r="M46" t="s">
         <v>72</v>
@@ -2730,8 +2866,11 @@
       <c r="P46">
         <v>44</v>
       </c>
-    </row>
-    <row r="47" spans="1:16">
+      <c r="Q46">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17">
       <c r="A47">
         <v>14126162</v>
       </c>
@@ -2749,7 +2888,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>86.015999999999991</v>
       </c>
       <c r="M47" t="s">
         <v>72</v>
@@ -2763,8 +2902,11 @@
       <c r="P47">
         <v>30</v>
       </c>
-    </row>
-    <row r="48" spans="1:16">
+      <c r="Q47">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17">
       <c r="A48">
         <v>14126163</v>
       </c>
@@ -2782,7 +2924,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>86.784000000000006</v>
       </c>
       <c r="M48" t="s">
         <v>72</v>
@@ -2793,8 +2935,11 @@
       <c r="P48">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:16">
+      <c r="Q48">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17">
       <c r="A49">
         <v>14126164</v>
       </c>
@@ -2812,7 +2957,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>79.679999999999993</v>
       </c>
       <c r="H49" t="s">
         <v>80</v>
@@ -2826,8 +2971,11 @@
       <c r="P49">
         <v>13</v>
       </c>
-    </row>
-    <row r="50" spans="1:16">
+      <c r="Q49">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17">
       <c r="A50">
         <v>14126165</v>
       </c>
@@ -2845,7 +2993,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>88.511999999999986</v>
       </c>
       <c r="M50" t="s">
         <v>72</v>
@@ -2856,8 +3004,11 @@
       <c r="P50">
         <v>43</v>
       </c>
-    </row>
-    <row r="51" spans="1:16">
+      <c r="Q50">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17">
       <c r="A51">
         <v>14126166</v>
       </c>
@@ -2875,7 +3026,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>84.47999999999999</v>
       </c>
       <c r="M51" t="s">
         <v>72</v>
@@ -2886,8 +3037,11 @@
       <c r="P51">
         <v>16</v>
       </c>
-    </row>
-    <row r="52" spans="1:16">
+      <c r="Q51">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17">
       <c r="A52">
         <v>14126169</v>
       </c>
@@ -2905,7 +3059,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>88.511999999999986</v>
       </c>
       <c r="M52" t="s">
         <v>72</v>
@@ -2916,8 +3070,11 @@
       <c r="P52">
         <v>61</v>
       </c>
-    </row>
-    <row r="53" spans="1:16">
+      <c r="Q52">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17">
       <c r="A53">
         <v>14126172</v>
       </c>
@@ -2935,7 +3092,7 @@
       </c>
       <c r="F53">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>81.599999999999994</v>
       </c>
       <c r="O53">
         <v>40</v>
@@ -2943,8 +3100,11 @@
       <c r="P53">
         <v>26</v>
       </c>
-    </row>
-    <row r="54" spans="1:16">
+      <c r="Q53">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17">
       <c r="A54">
         <v>14126173</v>
       </c>
@@ -2962,7 +3122,7 @@
       </c>
       <c r="F54">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>86.207999999999998</v>
       </c>
       <c r="M54" t="s">
         <v>72</v>
@@ -2973,8 +3133,11 @@
       <c r="P54">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" spans="1:16">
+      <c r="Q54">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17">
       <c r="A55">
         <v>14126175</v>
       </c>
@@ -2992,7 +3155,7 @@
       </c>
       <c r="F55">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>86.207999999999998</v>
       </c>
       <c r="M55" t="s">
         <v>72</v>
@@ -3003,8 +3166,11 @@
       <c r="P55">
         <v>37</v>
       </c>
-    </row>
-    <row r="56" spans="1:16">
+      <c r="Q55">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17">
       <c r="A56">
         <v>14126176</v>
       </c>
@@ -3022,7 +3188,7 @@
       </c>
       <c r="F56">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.24</v>
       </c>
       <c r="M56" t="s">
         <v>72</v>
@@ -3033,8 +3199,11 @@
       <c r="P56">
         <v>3</v>
       </c>
-    </row>
-    <row r="57" spans="1:16">
+      <c r="Q56">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17">
       <c r="A57">
         <v>14126177</v>
       </c>
@@ -3052,7 +3221,7 @@
       </c>
       <c r="F57">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>93.11999999999999</v>
       </c>
       <c r="M57" t="s">
         <v>72</v>
@@ -3063,8 +3232,11 @@
       <c r="P57">
         <v>9</v>
       </c>
-    </row>
-    <row r="58" spans="1:16">
+      <c r="Q57">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17">
       <c r="A58">
         <v>14126179</v>
       </c>
@@ -3082,7 +3254,7 @@
       </c>
       <c r="F58">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>82.56</v>
       </c>
       <c r="M58" t="s">
         <v>72</v>
@@ -3096,8 +3268,11 @@
       <c r="P58">
         <v>5</v>
       </c>
-    </row>
-    <row r="59" spans="1:16">
+      <c r="Q58">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17">
       <c r="A59">
         <v>14126181</v>
       </c>
@@ -3115,7 +3290,7 @@
       </c>
       <c r="F59">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>84.47999999999999</v>
       </c>
       <c r="M59" t="s">
         <v>72</v>
@@ -3126,8 +3301,11 @@
       <c r="P59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:16">
+      <c r="Q59">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17">
       <c r="A60">
         <v>14126185</v>
       </c>
@@ -3145,7 +3323,7 @@
       </c>
       <c r="F60">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.24</v>
       </c>
       <c r="M60" t="s">
         <v>72</v>
@@ -3156,8 +3334,11 @@
       <c r="P60">
         <v>45</v>
       </c>
-    </row>
-    <row r="61" spans="1:16">
+      <c r="Q60">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17">
       <c r="A61">
         <v>14126186</v>
       </c>
@@ -3175,7 +3356,7 @@
       </c>
       <c r="F61">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>73.92</v>
       </c>
       <c r="K61" t="s">
         <v>70</v>
@@ -3189,8 +3370,11 @@
       <c r="P61">
         <v>17</v>
       </c>
-    </row>
-    <row r="62" spans="1:16">
+      <c r="Q61">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17">
       <c r="A62">
         <v>14126187</v>
       </c>
@@ -3208,7 +3392,7 @@
       </c>
       <c r="F62">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>82.56</v>
       </c>
       <c r="I62" t="s">
         <v>67</v>
@@ -3222,8 +3406,11 @@
       <c r="P62">
         <v>49</v>
       </c>
-    </row>
-    <row r="63" spans="1:16">
+      <c r="Q62">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17">
       <c r="A63">
         <v>14126188</v>
       </c>
@@ -3241,7 +3428,7 @@
       </c>
       <c r="F63">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>87.36</v>
       </c>
       <c r="M63" t="s">
         <v>72</v>
@@ -3252,8 +3439,11 @@
       <c r="P63">
         <v>27</v>
       </c>
-    </row>
-    <row r="64" spans="1:16">
+      <c r="Q63">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17">
       <c r="A64">
         <v>14126192</v>
       </c>
@@ -3271,7 +3461,7 @@
       </c>
       <c r="F64">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>90.24</v>
       </c>
       <c r="M64" t="s">
         <v>72</v>
@@ -3282,8 +3472,11 @@
       <c r="P64">
         <v>24</v>
       </c>
-    </row>
-    <row r="65" spans="1:16">
+      <c r="Q64">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17">
       <c r="A65">
         <v>14126193</v>
       </c>
@@ -3301,7 +3494,7 @@
       </c>
       <c r="F65">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>88.32</v>
       </c>
       <c r="H65" t="s">
         <v>80</v>
@@ -3315,8 +3508,11 @@
       <c r="P65">
         <v>6</v>
       </c>
-    </row>
-    <row r="66" spans="1:16">
+      <c r="Q65">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17">
       <c r="A66">
         <v>14126196</v>
       </c>
@@ -3334,7 +3530,7 @@
       </c>
       <c r="F66">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>83.711999999999989</v>
       </c>
       <c r="I66" t="s">
         <v>68</v>
@@ -3348,8 +3544,11 @@
       <c r="P66">
         <v>25</v>
       </c>
-    </row>
-    <row r="67" spans="1:16">
+      <c r="Q66">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17">
       <c r="A67">
         <v>14126197</v>
       </c>
@@ -3366,8 +3565,8 @@
         <v>9</v>
       </c>
       <c r="F67">
-        <f t="shared" ref="F67" si="1">O67+Q67*0.6</f>
-        <v>43</v>
+        <f t="shared" ref="F67" si="1">(O67+Q67*0.6)*0.96</f>
+        <v>89.087999999999994</v>
       </c>
       <c r="M67" t="s">
         <v>72</v>
@@ -3377,6 +3576,9 @@
       </c>
       <c r="P67">
         <v>50</v>
+      </c>
+      <c r="Q67">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>